<commit_message>
Correcciones de ortografia, etc.
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/Indicaciones/IndicacionesFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/Indicaciones/IndicacionesFormulario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\API\Service.Catalog\wwwroot\layout\excel\Indicaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\Indicaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C58B359-ADE7-42D9-9CA3-38E571D3ADB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEA4ACA-7D73-432F-95EE-CB3AA5DEE89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Activo</t>
   </si>
   <si>
-    <t>Descripcíon</t>
-  </si>
-  <si>
     <t>{{Indicaciones.Clave}}</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>Área</t>
+  </si>
+  <si>
+    <t>Descripción</t>
   </si>
 </sst>
 </file>
@@ -200,21 +200,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A4281-45E9-4A26-88B5-8DB32AE336F4}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,11 +597,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -609,10 +609,10 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9"/>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
     </row>
@@ -623,10 +623,10 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9"/>
       <c r="D5" s="1"/>
       <c r="E5" s="2"/>
     </row>
@@ -635,12 +635,12 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
     </row>
@@ -651,10 +651,10 @@
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="B9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
     </row>
@@ -669,12 +669,12 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -685,29 +685,29 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -740,12 +740,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>